<commit_message>
IKD update: GaN CMOS 2026-01-29T07:25Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T85"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6835,6 +6835,1966 @@
       </c>
       <c r="T85" t="inlineStr"/>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>University of Slavonski Brod</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Tehnicki vjesnik - Technical Gazette</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Generation of SVPWM on FPGA to Control 3-Phase Inverter</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>International Journal for Research in Applied Science and Engineering Technology (IJRASET)</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>International Journal for Research in Applied Science and Engineering Technology</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Vandana, Nimma</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>10.22214/ijraset.2026.76782</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.22214/ijraset.2026.76782</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>Generation of SVPWM on FPGA to Control 3-Phase Inverter</t>
+        </is>
+      </c>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>University of Slavonski Brod</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Tehnicki vjesnik - Technical Gazette</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Charge vertical diffusion control of threshold voltage behavior in GaN MIS-HEMTs under bias temperature instability (BTI)</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Materials Science in Semiconductor Processing</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Yang, YeonSil; An, Do gyun; Lee, Kang Hee; Heo, Junseok; Kim, Jang Hyun</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>10.1016/j.mssp.2025.110190</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mssp.2025.110190</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>Charge vertical diffusion control of threshold voltage behavior in GaN MIS-HEMTs under bias temperature instability (BTI)</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Nuclear Engineering and Technology</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Chen, De-Xin; Wang, Ying; Cui, Wan-zhao; Song, Yan-xing; Cao, Fei</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Performance enhancement in 3D transistors: A TCAD simulation-based study of FinFETs and GAAFETs with novel source-drain extensions</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Micro and Nanostructures</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Li, Man; Huang, Yifan; Xiao, Wei; Wang, Mingxiang; Guo, Yeye; Zhang, Dongli; Wang, Huaisheng; Shen, Chen; Gong, Ding</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>10.1016/j.micrna.2025.208473</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.micrna.2025.208473</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>Performance enhancement in 3D transistors: A TCAD simulation-based study of FinFETs and GAAFETs with novel source-drain extensions</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>IEEE Transactions on Power Electronics</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Yang, Xin; Yang, Zineng; Porter, Matthew; Shao, Linbo; Zhang, Yuhao</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Electrostatic discharge power-rail clamp circuit with silicon-controlled rectifier and MOSFET hybrid clamping device</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Microelectronics Journal</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Yue, Yaping; Wu, Ruizhen; Hou, Ronghui; Yang, Yuan</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>10.1016/j.mejo.2025.107008</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mejo.2025.107008</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>Electrostatic discharge power-rail clamp circuit with silicon-controlled rectifier and MOSFET hybrid clamping device</t>
+        </is>
+      </c>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Study on the performance of closed-loop control system considering bond wires aging of SiC MOSFET</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Microelectronics Journal</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Du, Mingxing; Wang, Shaoxiang; Yang, Jianxiong; Huang, Xiyuan; Qiao, Haotian</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>10.1016/j.mejo.2025.106998</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mejo.2025.106998</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>Study on the performance of closed-loop control system considering bond wires aging of SiC MOSFET</t>
+        </is>
+      </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>IEEE Transactions on Power Electronics</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Yang, Xin; Yang, Zineng; Porter, Matthew; Shao, Linbo; Zhang, Yuhao</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>IEEE Transactions on Power Electronics</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Yang, Xin; Yang, Zineng; Porter, Matthew; Shao, Linbo; Zhang, Yuhao</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Nuclear Engineering and Technology</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Chen, De-Xin; Wang, Ying; Cui, Wan-zhao; Song, Yan-xing; Cao, Fei</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Performance enhancement in 3D transistors: A TCAD simulation-based study of FinFETs and GAAFETs with novel source-drain extensions</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Micro and Nanostructures</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Li, Man; Huang, Yifan; Xiao, Wei; Wang, Mingxiang; Guo, Yeye; Zhang, Dongli; Wang, Huaisheng; Shen, Chen; Gong, Ding</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>10.1016/j.micrna.2025.208473</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.micrna.2025.208473</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>Performance enhancement in 3D transistors: A TCAD simulation-based study of FinFETs and GAAFETs with novel source-drain extensions</t>
+        </is>
+      </c>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Electrostatic discharge power-rail clamp circuit with silicon-controlled rectifier and MOSFET hybrid clamping device</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Microelectronics Journal</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Yue, Yaping; Wu, Ruizhen; Hou, Ronghui; Yang, Yuan</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>10.1016/j.mejo.2025.107008</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mejo.2025.107008</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>Electrostatic discharge power-rail clamp circuit with silicon-controlled rectifier and MOSFET hybrid clamping device</t>
+        </is>
+      </c>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Study on the performance of closed-loop control system considering bond wires aging of SiC MOSFET</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Microelectronics Journal</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Du, Mingxing; Wang, Shaoxiang; Yang, Jianxiong; Huang, Xiyuan; Qiao, Haotian</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>10.1016/j.mejo.2025.106998</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mejo.2025.106998</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>Study on the performance of closed-loop control system considering bond wires aging of SiC MOSFET</t>
+        </is>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Design and characterization of 2-GaN MIS-HEMT integrated cascode power module</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Microelectronic Engineering</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Elangovan, Surya; Cheng, Stone; Chang, Edward Yi; Rawat, Tejender Singh; Hsiao, Yi-Kai; Tu, Chang-Ching; Kuo, Hao-Chung</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>10.1016/j.mee.2025.112439</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mee.2025.112439</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>Design and characterization of 2-GaN MIS-HEMT integrated cascode power module</t>
+        </is>
+      </c>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>IEEE Transactions on Power Electronics</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Yang, Xin; Yang, Zineng; Porter, Matthew; Shao, Linbo; Zhang, Yuhao</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/tpel.2025.3601008</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>First Characterization of Si IGBT, SiC MOSFET, and GaN HEMT at Deep Cryogenic Temperatures Down to 10 Millikelvins</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Charge vertical diffusion control of threshold voltage behavior in GaN MIS-HEMTs under bias temperature instability (BTI)</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Materials Science in Semiconductor Processing</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Yang, YeonSil; An, Do gyun; Lee, Kang Hee; Heo, Junseok; Kim, Jang Hyun</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>10.1016/j.mssp.2025.110190</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mssp.2025.110190</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>Charge vertical diffusion control of threshold voltage behavior in GaN MIS-HEMTs under bias temperature instability (BTI)</t>
+        </is>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Nuclear Engineering and Technology</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Chen, De-Xin; Wang, Ying; Cui, Wan-zhao; Song, Yan-xing; Cao, Fei</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.net.2025.103979</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>Dual voltage-dependent mechanisms of single-event leakage current in SiC trench MOSFETs: Heavy-Ion irradiation and TCAD simulation study</t>
+        </is>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>University of Slavonski Brod</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Tehnicki vjesnik - Technical Gazette</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Generation of SVPWM on FPGA to Control 3-Phase Inverter</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>International Journal for Research in Applied Science and Engineering Technology (IJRASET)</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>International Journal for Research in Applied Science and Engineering Technology</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Vandana, Nimma</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>10.22214/ijraset.2026.76782</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.22214/ijraset.2026.76782</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>Generation of SVPWM on FPGA to Control 3-Phase Inverter</t>
+        </is>
+      </c>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>A 95.3% 12-Class, 108-nJ/Inference Keyword Spotting Chip With Hybrid FFT-BFNet Architecture and Exponent-Aware Nonuniform Quantization in 65-nm CMOS</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>IEEE Transactions on Very Large Scale Integration (VLSI) Systems</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Fu, Zongpei; Lin, Kaixiang; Zhao, Xiaojin; Ge, Lei; Ye, Wenbin</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>10.1109/tvlsi.2025.3632791</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/tvlsi.2025.3632791</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>A 95.3% 12-Class, 108-nJ/Inference Keyword Spotting Chip With Hybrid FFT-BFNet Architecture and Exponent-Aware Nonuniform Quantization in 65-nm CMOS</t>
+        </is>
+      </c>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>University of Slavonski Brod</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Tehnicki vjesnik - Technical Gazette</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.17559/tv-20250411002584</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>Symmetrical and High-Speed CMOS Inverter Design Using Hybrid PSOGSA Optimization Algorithm</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Integrated DNA logic gate-driven cell membrane confined amplification system for imaging cellular events</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Nano Today</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Guo, Zhenzhen; Qiu, Yue; Wang, Yang; Zhang, Jiali; Jiang, Xiaotong; Wang, Danyu; Yi, Hua; Huang, Mengyu; Chen, Peiru; Zhang, Fangmei; Liang, Yan; Chen, Fengming</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>10.1016/j.nantod.2025.102934</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.nantod.2025.102934</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>Reliability</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>Integrated DNA logic gate-driven cell membrane confined amplification system for imaging cellular events</t>
+        </is>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Optimization of central source contact length to mitigate temperature variation and thermal crosstalk in multi-finger AlGaN/GaN HEMTs: Reliability-based simulation</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Materials Science in Semiconductor Processing</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Lim, Chae-Yun; Lee, Jae-Hun; Kim, Tae-Sung; Won, Young-Hyun; Min, Byoung-Gue; Kang, Dong Min; Kim, Hyun-Seok</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>10.1016/j.mssp.2025.110184</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mssp.2025.110184</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>Optimization of central source contact length to mitigate temperature variation and thermal crosstalk in multi-finger AlGaN/GaN HEMTs: Reliability-based simulation</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Optimization of central source contact length to mitigate temperature variation and thermal crosstalk in multi-finger AlGaN/GaN HEMTs: Reliability-based simulation</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Materials Science in Semiconductor Processing</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Lim, Chae-Yun; Lee, Jae-Hun; Kim, Tae-Sung; Won, Young-Hyun; Min, Byoung-Gue; Kang, Dong Min; Kim, Hyun-Seok</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>10.1016/j.mssp.2025.110184</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.mssp.2025.110184</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>Optimization of central source contact length to mitigate temperature variation and thermal crosstalk in multi-finger AlGaN/GaN HEMTs: Reliability-based simulation</t>
+        </is>
+      </c>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="T111" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-01-30T23:29Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T111"/>
+  <dimension ref="A1:T112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8795,6 +8795,82 @@
       </c>
       <c r="T111" t="inlineStr"/>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Low Threshold Voltage Temperature Coefficient Due to Thermal Stress in GaN-on-Diamond HEMTs</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>IEEE Electron Device Letters</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Huang, Lei; Wu, Qingzhi; Mao, Shuman; Kong, Yuechan; Chen, Tangsheng; Xu, Yuehang</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>10.1109/led.2025.3646340</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1109/led.2025.3646340</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>Electrostatics</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>Low Threshold Voltage Temperature Coefficient Due to Thermal Stress in GaN-on-Diamond HEMTs</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="T112" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-01-31T23:27Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T112"/>
+  <dimension ref="A1:T118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8871,6 +8871,454 @@
       </c>
       <c r="T112" t="inlineStr"/>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>A CMOS Measurement-Collapse Primitive for Ephemeral Secrets in Post-Quantum Cryptography</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>III, Francis X. Cunnane</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.176463742.23048082/v3</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.176463742.23048082/v3</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>A CMOS Measurement-Collapse Primitive for Ephemeral Secrets in Post-Quantum Cryptography</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>A CMOS Measurement-Collapse Primitive for Ephemeral Secrets in Post-Quantum Cryptography</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>III, Francis X. Cunnane</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.176463742.23048082/v3</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.176463742.23048082/v3</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>A CMOS Measurement-Collapse Primitive for Ephemeral Secrets in Post-Quantum Cryptography</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>The Electrochemical Society</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>ECS Journal of Solid State Science and Technology</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Xu, Fan; Dai, Ming; Duan, JunFeng; Zhu, Shengnan; Qiao, Yuan; Yi, Bo; Cheng, Junji; Yang, Hongqiang</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>The Electrochemical Society</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>ECS Journal of Solid State Science and Technology</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Xu, Fan; Dai, Ming; Duan, JunFeng; Zhu, Shengnan; Qiao, Yuan; Yi, Bo; Cheng, Junji; Yang, Hongqiang</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>The Electrochemical Society</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>ECS Journal of Solid State Science and Technology</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Xu, Fan; Dai, Ming; Duan, JunFeng; Zhu, Shengnan; Qiao, Yuan; Yi, Bo; Cheng, Junji; Yang, Hongqiang</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>The Electrochemical Society</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>ECS Journal of Solid State Science and Technology</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Xu, Fan; Dai, Ming; Duan, JunFeng; Zhu, Shengnan; Qiao, Yuan; Yi, Bo; Cheng, Junji; Yang, Hongqiang</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1149/2162-8777/ae3fce</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>TCAD Demonstration of a High-Voltage Lateral Double-RESURF-VLD β-Ga2O3 MISFET with p-type Diamond for Ultra-Low Ron,sp</t>
+        </is>
+      </c>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="T118" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>